<commit_message>
update protein lincs id import & sample data
</commit_message>
<xml_diff>
--- a/sampledata/sample_antibodies.xlsx
+++ b/sampledata/sample_antibodies.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="Excel_BuiltIn_Print_Area" vbProcedure="false">{#NAME?}</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="Excel_BuiltIn_Print_Area" vbProcedure="false">{#name?}</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Excel_BuiltIn_Sheet_Title" vbProcedure="false">"Sheet1"</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -123,7 +123,7 @@
     <t>natural</t>
   </si>
   <si>
-    <t>HMSL201294</t>
+    <t>LSM-200001</t>
   </si>
   <si>
     <t>Homo sapiens</t>
@@ -171,7 +171,7 @@
     <t>AB_10892861</t>
   </si>
   <si>
-    <t>HMSL201295</t>
+    <t>LSM-200002</t>
   </si>
   <si>
     <t>Monoclonal antibody is produced by immunizing animals with a synthetic peptide corresponding to residues near the carboxy terminus of human p21 protein. (source: Cell Signaling Technology)</t>
@@ -195,7 +195,7 @@
     <t>not available</t>
   </si>
   <si>
-    <t>HMSL201296</t>
+    <t>LSM-200003</t>
   </si>
   <si>
     <t>Monoclonal antibody is produced by immunizing animals with recombinant protein specific to the amino terminus of human Ki-67 protein. (source: Cell Signaling Technology)</t>
@@ -216,7 +216,7 @@
     <t>D20B12</t>
   </si>
   <si>
-    <t>HMSL201297</t>
+    <t>LSM-200004</t>
   </si>
   <si>
     <t>Monoclonal antibody is produced by immunizing animals with a synthetic phosphopeptide corresponding to residues surrounding Ser807/811 of human Rb protein. (source: Cell Signaling Technology)</t>
@@ -237,7 +237,7 @@
     <t>AB_916160</t>
   </si>
   <si>
-    <t>HMSL201298</t>
+    <t>LSM-200005</t>
   </si>
   <si>
     <t>Monoclonal antibody is produced by immunizing animals with a synthetic phosphopeptide corresponding to residues surrounding Ser235 and Ser236 of human ribosomal protein S6. (source: Cell Signaling Technology)</t>
@@ -258,7 +258,7 @@
     <t>AB_10695861</t>
   </si>
   <si>
-    <t>HMSL201299</t>
+    <t>LSM-200006</t>
   </si>
   <si>
     <t>Monoclonal antibody is produced by immunizing animals with a synthetic phosphopeptide corresponding to residues surrounding Ser240 and Ser244 of human ribosomal protein S6. (source: Cell Signaling Technology)</t>
@@ -303,6 +303,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -324,6 +325,7 @@
       <color rgb="FF800000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -331,6 +333,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -338,17 +341,20 @@
       <color rgb="FF800000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -478,7 +484,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>